<commit_message>
jsf validation -> bean validation #37
</commit_message>
<xml_diff>
--- a/src/main/resources/template/doc/sit_simple/書式定義書.xlsx
+++ b/src/main/resources/template/doc/sit_simple/書式定義書.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\yuichi.kuwahara\Dropbox\NetBeansProjects2\sit-archetype\sit\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\sit\netbeans-workspace\workspace-sit-archetype\sit-core\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="120" windowWidth="19400" windowHeight="8490"/>
+    <workbookView xWindow="600" yWindow="120" windowWidth="19400" windowHeight="8490" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="表紙" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="53">
   <si>
     <t>表示書式</t>
     <rPh sb="0" eb="2">
@@ -358,6 +358,10 @@
       <t>シュウリョウ</t>
     </rPh>
     <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>AlphaNumeric</t>
+    <phoneticPr fontId="2"/>
   </si>
 </sst>
 </file>
@@ -989,7 +993,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13"/>
   <cols>
@@ -1005,7 +1009,7 @@
       </c>
       <c r="G2" s="27" t="str">
         <f ca="1">CELL("filename",G2)</f>
-        <v>D:\Users\yuichi.kuwahara\Dropbox\NetBeansProjects2\sit-archetype\sit\doc\[書式定義書.xlsx]表紙</v>
+        <v>D:\sit\netbeans-workspace\workspace-sit-archetype\sit-core\doc\[書式定義書.xlsx]表紙</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -1014,7 +1018,7 @@
       </c>
       <c r="G3" s="27">
         <f ca="1">FIND("[",G2)</f>
-        <v>74</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:7" s="12" customFormat="1">
@@ -1027,7 +1031,7 @@
       </c>
       <c r="G4" s="27">
         <f ca="1">FIND(".xlsx",G2)</f>
-        <v>80</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:7" s="12" customFormat="1">
@@ -1131,7 +1135,7 @@
     <row r="23" spans="1:4" s="12" customFormat="1">
       <c r="A23" s="33">
         <f ca="1">MAX(更新履歴!C5:C15)</f>
-        <v>41375</v>
+        <v>41612</v>
       </c>
       <c r="B23" s="32"/>
       <c r="C23" s="32"/>
@@ -1330,7 +1334,7 @@
       </c>
       <c r="C5" s="20">
         <f ca="1">TODAY()-31</f>
-        <v>41375</v>
+        <v>41612</v>
       </c>
       <c r="D5" s="21" t="s">
         <v>43</v>
@@ -1413,7 +1417,9 @@
   </sheetPr>
   <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13"/>
   <cols>
@@ -1578,7 +1584,7 @@
         <v>11</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>11</v>
+        <v>52</v>
       </c>
       <c r="K7" s="4" t="s">
         <v>24</v>

</xml_diff>